<commit_message>
Updated results after updating code
</commit_message>
<xml_diff>
--- a/results_table.xlsx
+++ b/results_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/ranik_ntnu_no/Documents/Research/datasett_aarsregnskaper/code_for_github/datasett_aarsregnskaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_23F921EDF1334F3CE42B84DEC470F3AA7452AF73" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8CFC7F1-BAF5-40F2-95EB-6DEB4224B8B0}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_23F921ED652B4B289C2A843ED471C5667552AF72" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDDC0B7C-5994-4EEF-8CB3-F3AA6DFE9303}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,8 +103,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -171,8 +171,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -515,7 +515,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,34 +561,34 @@
         <v>10</v>
       </c>
       <c r="B2" s="2">
-        <v>1.6382593130835481</v>
+        <v>1.6411739265269689</v>
       </c>
       <c r="C2" s="2">
-        <v>1.664367080178387</v>
+        <v>1.667872126451722</v>
       </c>
       <c r="D2" s="2">
-        <v>1.694745393646611</v>
+        <v>1.698460096865025</v>
       </c>
       <c r="E2" s="2">
-        <v>1.7450286661890331</v>
+        <v>1.7489736885111791</v>
       </c>
       <c r="F2" s="2">
-        <v>1.80959141409444</v>
+        <v>1.8132517678640081</v>
       </c>
       <c r="G2" s="2">
-        <v>1.8334241630836841</v>
+        <v>1.836963622479314</v>
       </c>
       <c r="H2" s="2">
-        <v>1.7671261792670281</v>
+        <v>1.770539582102479</v>
       </c>
       <c r="I2" s="2">
-        <v>1.7892979879688331</v>
+        <v>1.7921506359970809</v>
       </c>
       <c r="J2" s="2">
-        <v>1.771006938530082</v>
+        <v>1.7741962232528019</v>
       </c>
       <c r="K2" s="2">
-        <v>1.779004722457604</v>
+        <v>1.781968483630171</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -596,34 +596,34 @@
         <v>11</v>
       </c>
       <c r="B3" s="2">
-        <v>0.57864171272409293</v>
+        <v>0.57976862227244741</v>
       </c>
       <c r="C3" s="2">
-        <v>0.56378540190619175</v>
+        <v>0.56502024272712859</v>
       </c>
       <c r="D3" s="2">
-        <v>0.56483306590043747</v>
+        <v>0.56589905261336693</v>
       </c>
       <c r="E3" s="2">
-        <v>0.5914951458144162</v>
+        <v>0.59280069342795227</v>
       </c>
       <c r="F3" s="2">
-        <v>0.57797448609765345</v>
+        <v>0.57960263946486501</v>
       </c>
       <c r="G3" s="2">
-        <v>0.5641371759636209</v>
+        <v>0.56617500368478701</v>
       </c>
       <c r="H3" s="2">
-        <v>0.59458628680446535</v>
+        <v>0.59684556151023394</v>
       </c>
       <c r="I3" s="2">
-        <v>0.57985605153666786</v>
+        <v>0.5818486751421702</v>
       </c>
       <c r="J3" s="2">
-        <v>0.59211939897438859</v>
+        <v>0.59368051374948827</v>
       </c>
       <c r="K3" s="2">
-        <v>0.57839355933792136</v>
+        <v>0.58006539990416672</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -631,34 +631,34 @@
         <v>12</v>
       </c>
       <c r="B4" s="2">
-        <v>0.85062220095552876</v>
+        <v>0.85205721154901215</v>
       </c>
       <c r="C4" s="2">
-        <v>0.86437927151140082</v>
+        <v>0.86593322804584227</v>
       </c>
       <c r="D4" s="2">
-        <v>0.88249022767577234</v>
+        <v>0.88511818200996517</v>
       </c>
       <c r="E4" s="2">
-        <v>0.92499078283497549</v>
+        <v>0.92774113303031502</v>
       </c>
       <c r="F4" s="2">
-        <v>0.88589024647689929</v>
+        <v>0.8893464520171549</v>
       </c>
       <c r="G4" s="2">
-        <v>0.95840278702170967</v>
+        <v>0.96202048112459981</v>
       </c>
       <c r="H4" s="2">
-        <v>0.97605954483972646</v>
+        <v>0.97873490499882398</v>
       </c>
       <c r="I4" s="2">
-        <v>0.96852691690890025</v>
+        <v>0.97020051801816098</v>
       </c>
       <c r="J4" s="2">
-        <v>1.0426340154923901</v>
+        <v>1.043689769745543</v>
       </c>
       <c r="K4" s="2">
-        <v>0.98008591428092395</v>
+        <v>0.98135672311022693</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -666,34 +666,34 @@
         <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>-1.0276088716086811</v>
+        <v>-1.028165284423548</v>
       </c>
       <c r="C5" s="2">
-        <v>-0.98374514730251583</v>
+        <v>-0.98406695399440447</v>
       </c>
       <c r="D5" s="2">
-        <v>-0.95107993826625359</v>
+        <v>-0.95132442576713139</v>
       </c>
       <c r="E5" s="2">
-        <v>-0.91909210461511803</v>
+        <v>-0.91926426512542581</v>
       </c>
       <c r="F5" s="2">
-        <v>-0.89282061645758437</v>
+        <v>-0.89313580038201146</v>
       </c>
       <c r="G5" s="2">
-        <v>-0.86247237657372844</v>
+        <v>-0.86288803354203225</v>
       </c>
       <c r="H5" s="2">
-        <v>-0.83244511867089688</v>
+        <v>-0.83249320049629727</v>
       </c>
       <c r="I5" s="2">
-        <v>-0.8161498636534239</v>
+        <v>-0.81681163003256885</v>
       </c>
       <c r="J5" s="2">
-        <v>-0.83126047194798536</v>
+        <v>-0.83180590472406601</v>
       </c>
       <c r="K5" s="2">
-        <v>-0.80208576506890272</v>
+        <v>-0.80277422479186933</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -701,34 +701,34 @@
         <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>3.2207313708809902</v>
+        <v>3.227336134385272</v>
       </c>
       <c r="C6" s="2">
-        <v>3.1959903305435158</v>
+        <v>3.203663840100281</v>
       </c>
       <c r="D6" s="2">
-        <v>3.3092705401691238</v>
+        <v>3.317941395471216</v>
       </c>
       <c r="E6" s="2">
-        <v>3.4089933690849081</v>
+        <v>3.4184220094171049</v>
       </c>
       <c r="F6" s="2">
-        <v>3.6211954291790991</v>
+        <v>3.6295453287968789</v>
       </c>
       <c r="G6" s="2">
-        <v>3.9834917691058438</v>
+        <v>3.992001656828136</v>
       </c>
       <c r="H6" s="2">
-        <v>4.1747735426024866</v>
+        <v>4.1826640884016433</v>
       </c>
       <c r="I6" s="2">
-        <v>4.3875646715708552</v>
+        <v>4.3943882785342439</v>
       </c>
       <c r="J6" s="2">
-        <v>4.3726882734247026</v>
+        <v>4.3807731143531718</v>
       </c>
       <c r="K6" s="2">
-        <v>4.3466689917072694</v>
+        <v>4.3546536610317457</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -736,34 +736,34 @@
         <v>15</v>
       </c>
       <c r="B7" s="2">
-        <v>1.0262997655273891</v>
+        <v>0.99353315506057538</v>
       </c>
       <c r="C7" s="2">
-        <v>1.3880019914339421</v>
+        <v>1.3536146363070789</v>
       </c>
       <c r="D7" s="2">
-        <v>1.4322302137320579</v>
+        <v>1.398595998273352</v>
       </c>
       <c r="E7" s="2">
-        <v>2.5802518675777519</v>
+        <v>2.5440079610487061</v>
       </c>
       <c r="F7" s="2">
-        <v>3.1479149473927399</v>
+        <v>3.1076673136929869</v>
       </c>
       <c r="G7" s="2">
-        <v>2.8528721491239089</v>
+        <v>2.8103074399245029</v>
       </c>
       <c r="H7" s="2">
-        <v>2.9260164983252359</v>
+        <v>2.8949515819528719</v>
       </c>
       <c r="I7" s="2">
-        <v>2.8421041576924981</v>
+        <v>2.8269330952668872</v>
       </c>
       <c r="J7" s="2">
-        <v>2.2523574033629399</v>
+        <v>2.2447163298704238</v>
       </c>
       <c r="K7" s="2">
-        <v>2.4305954643619341</v>
+        <v>2.4225991781272729</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -771,34 +771,34 @@
         <v>16</v>
       </c>
       <c r="B8" s="2">
-        <v>1.047133200671633</v>
+        <v>1.0463420871357729</v>
       </c>
       <c r="C8" s="2">
-        <v>1.0267507074589219</v>
+        <v>1.025827748558221</v>
       </c>
       <c r="D8" s="2">
-        <v>1.017420976031947</v>
+        <v>1.016852077790918</v>
       </c>
       <c r="E8" s="2">
-        <v>0.9423455766106601</v>
+        <v>0.94156566131389985</v>
       </c>
       <c r="F8" s="2">
-        <v>0.87634966642353263</v>
+        <v>0.87475556046395164</v>
       </c>
       <c r="G8" s="2">
-        <v>0.80869315839642431</v>
+        <v>0.8068599929347543</v>
       </c>
       <c r="H8" s="2">
-        <v>0.71156267265609785</v>
+        <v>0.70904690310966334</v>
       </c>
       <c r="I8" s="2">
-        <v>0.67195471316585631</v>
+        <v>0.66871591444463641</v>
       </c>
       <c r="J8" s="2">
-        <v>0.64729714016206008</v>
+        <v>0.64470825705916013</v>
       </c>
       <c r="K8" s="2">
-        <v>0.68191162160824648</v>
+        <v>0.67927339409407972</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -806,34 +806,34 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>-0.33587659897616651</v>
+        <v>-0.33566701355408579</v>
       </c>
       <c r="C9" s="2">
-        <v>-0.34414166572758242</v>
+        <v>-0.34388727595670499</v>
       </c>
       <c r="D9" s="2">
-        <v>-0.33692086982269531</v>
+        <v>-0.33660172772579172</v>
       </c>
       <c r="E9" s="2">
-        <v>-0.3502704650831554</v>
+        <v>-0.34997800973909787</v>
       </c>
       <c r="F9" s="2">
-        <v>-0.36950099396979552</v>
+        <v>-0.36924624539847328</v>
       </c>
       <c r="G9" s="2">
-        <v>-0.38813370907606531</v>
+        <v>-0.38787451274335327</v>
       </c>
       <c r="H9" s="2">
-        <v>-0.39932015981935581</v>
+        <v>-0.39904302831325278</v>
       </c>
       <c r="I9" s="2">
-        <v>-0.42049498769789118</v>
+        <v>-0.42046480490998678</v>
       </c>
       <c r="J9" s="2">
-        <v>-0.4216951734755025</v>
+        <v>-0.42164367233483518</v>
       </c>
       <c r="K9" s="2">
-        <v>-0.40454953744857708</v>
+        <v>-0.40449228804044057</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -841,34 +841,34 @@
         <v>18</v>
       </c>
       <c r="B10" s="2">
-        <v>1.7570408525220741E-2</v>
+        <v>1.8181953837443809E-2</v>
       </c>
       <c r="C10" s="2">
-        <v>1.4339264470942409E-2</v>
+        <v>1.505055270002828E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>7.3824118380972879E-3</v>
+        <v>8.0672488724928913E-3</v>
       </c>
       <c r="E10" s="2">
-        <v>1.3299949493955521E-2</v>
+        <v>1.4034536234985569E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>6.1018087883297064E-3</v>
+        <v>6.6473918946292768E-3</v>
       </c>
       <c r="G10" s="2">
-        <v>2.7221114646438539E-3</v>
+        <v>3.2705899223109199E-3</v>
       </c>
       <c r="H10" s="2">
-        <v>-1.167564954222771E-3</v>
+        <v>-5.9453641947568336E-4</v>
       </c>
       <c r="I10" s="2">
-        <v>-1.2992495689128331E-2</v>
+        <v>-1.243703551319853E-2</v>
       </c>
       <c r="J10" s="2">
-        <v>-3.1837603489547672E-2</v>
+        <v>-3.1132091544909191E-2</v>
       </c>
       <c r="K10" s="2">
-        <v>-4.1027632294125108E-2</v>
+        <v>-4.0395006709870222E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -876,34 +876,34 @@
         <v>19</v>
       </c>
       <c r="B11" s="2">
-        <v>-5.2375190628093176</v>
+        <v>-5.2404351806069771</v>
       </c>
       <c r="C11" s="2">
-        <v>-5.2065992043724618</v>
+        <v>-5.2100334311689949</v>
       </c>
       <c r="D11" s="2">
-        <v>-5.3414953359358286</v>
+        <v>-5.3462435924122627</v>
       </c>
       <c r="E11" s="2">
-        <v>-5.4018901552788048</v>
+        <v>-5.4068216679950361</v>
       </c>
       <c r="F11" s="2">
-        <v>-5.4092339838860344</v>
+        <v>-5.4135346858151037</v>
       </c>
       <c r="G11" s="2">
-        <v>-5.4330765175525277</v>
+        <v>-5.4373641695459041</v>
       </c>
       <c r="H11" s="2">
-        <v>-5.4424738116317979</v>
+        <v>-5.4458977144080549</v>
       </c>
       <c r="I11" s="2">
-        <v>-5.4190722795776978</v>
+        <v>-5.4211222498342932</v>
       </c>
       <c r="J11" s="2">
-        <v>-5.432105991035538</v>
+        <v>-5.434736018369648</v>
       </c>
       <c r="K11" s="2">
-        <v>-5.4125290756128788</v>
+        <v>-5.4152423325676384</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -911,34 +911,34 @@
         <v>20</v>
       </c>
       <c r="B12" s="2">
-        <v>0.85563139048033332</v>
+        <v>0.85573675100067004</v>
       </c>
       <c r="C12" s="2">
-        <v>0.85761693006012452</v>
+        <v>0.85773064727643067</v>
       </c>
       <c r="D12" s="2">
-        <v>0.85829095769426222</v>
+        <v>0.85848441513750184</v>
       </c>
       <c r="E12" s="2">
-        <v>0.86099553240961169</v>
+        <v>0.86119631930388285</v>
       </c>
       <c r="F12" s="2">
-        <v>0.86268488376948826</v>
+        <v>0.86280632349525188</v>
       </c>
       <c r="G12" s="2">
-        <v>0.86262499640466916</v>
+        <v>0.86275591869981272</v>
       </c>
       <c r="H12" s="2">
-        <v>0.86324532903942541</v>
+        <v>0.86331819516928354</v>
       </c>
       <c r="I12" s="2">
-        <v>0.86360227525266753</v>
+        <v>0.86366631572375652</v>
       </c>
       <c r="J12" s="2">
-        <v>0.86230886663713546</v>
+        <v>0.86243397304631564</v>
       </c>
       <c r="K12" s="2">
-        <v>0.86140572780056013</v>
+        <v>0.86154233992522722</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -946,34 +946,34 @@
         <v>21</v>
       </c>
       <c r="B13" s="2">
-        <v>0.85713523352945131</v>
+        <v>0.85731228447012064</v>
       </c>
       <c r="C13" s="2">
-        <v>0.86047550529813843</v>
+        <v>0.86067727468320498</v>
       </c>
       <c r="D13" s="2">
-        <v>0.86416772580455115</v>
+        <v>0.86437038851687853</v>
       </c>
       <c r="E13" s="2">
-        <v>0.86386717512311395</v>
+        <v>0.86377979896211154</v>
       </c>
       <c r="F13" s="2">
-        <v>0.85846758811106694</v>
+        <v>0.85866019574214181</v>
       </c>
       <c r="G13" s="2">
-        <v>0.86334195397273861</v>
+        <v>0.8632717590963056</v>
       </c>
       <c r="H13" s="2">
-        <v>0.86677054990988189</v>
+        <v>0.86690496064160205</v>
       </c>
       <c r="I13" s="2">
-        <v>0.86027360158546873</v>
+        <v>0.86048001992952783</v>
       </c>
       <c r="J13" s="2">
-        <v>0.85596115479979573</v>
+        <v>0.85619201266478917</v>
       </c>
       <c r="K13" s="2">
-        <v>0.86834594997113157</v>
+        <v>0.86856724383201034</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -981,34 +981,34 @@
         <v>22</v>
       </c>
       <c r="B14" s="2">
-        <v>0.1933302522425159</v>
+        <v>0.1934703977634428</v>
       </c>
       <c r="C14" s="2">
-        <v>0.19316751171380181</v>
+        <v>0.19331531764831239</v>
       </c>
       <c r="D14" s="2">
-        <v>0.19432098319971949</v>
+        <v>0.19453887496887981</v>
       </c>
       <c r="E14" s="2">
-        <v>0.19824016055255461</v>
+        <v>0.1984670353539123</v>
       </c>
       <c r="F14" s="2">
-        <v>0.20045243761083509</v>
+        <v>0.20060768975658719</v>
       </c>
       <c r="G14" s="2">
-        <v>0.2016344706644371</v>
+        <v>0.20180714747620249</v>
       </c>
       <c r="H14" s="2">
-        <v>0.19880395546500571</v>
+        <v>0.19891427221552671</v>
       </c>
       <c r="I14" s="2">
-        <v>0.19890687003284571</v>
+        <v>0.19898659053479609</v>
       </c>
       <c r="J14" s="2">
-        <v>0.19802004479439739</v>
+        <v>0.19816021021328051</v>
       </c>
       <c r="K14" s="2">
-        <v>0.19686925651628831</v>
+        <v>0.19701443397837509</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1016,34 +1016,34 @@
         <v>23</v>
       </c>
       <c r="B15" s="3">
-        <v>108762</v>
+        <v>109048</v>
       </c>
       <c r="C15" s="3">
-        <v>111512</v>
+        <v>111831</v>
       </c>
       <c r="D15" s="3">
-        <v>116084</v>
+        <v>116429</v>
       </c>
       <c r="E15" s="3">
-        <v>120521</v>
+        <v>120856</v>
       </c>
       <c r="F15" s="3">
-        <v>124835</v>
+        <v>125207</v>
       </c>
       <c r="G15" s="3">
-        <v>129259</v>
+        <v>129627</v>
       </c>
       <c r="H15" s="3">
-        <v>133823</v>
+        <v>134208</v>
       </c>
       <c r="I15" s="3">
-        <v>139063</v>
+        <v>139450</v>
       </c>
       <c r="J15" s="3">
-        <v>143256</v>
+        <v>143671</v>
       </c>
       <c r="K15" s="3">
-        <v>145387</v>
+        <v>145830</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1060,16 +1060,16 @@
         <v>1688</v>
       </c>
       <c r="E16" s="3">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="F16" s="3">
         <v>1601</v>
       </c>
       <c r="G16" s="3">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="H16" s="3">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="I16" s="3">
         <v>1746</v>

</xml_diff>

<commit_message>
Added code for making LASSO path on training sets
</commit_message>
<xml_diff>
--- a/results_table.xlsx
+++ b/results_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/ranik_ntnu_no/Documents/Research/datasett_aarsregnskaper/code_for_github/datasett_aarsregnskaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_23F921ED652B4B289C2A843ED471C5667552AF72" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDDC0B7C-5994-4EEF-8CB3-F3AA6DFE9303}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_23F921EDEB23C91AB82A84497433F36A7552AF72" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB795F55-5B6A-4330-A0F8-43E8FE8A4536}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,14 +514,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -946,34 +944,34 @@
         <v>21</v>
       </c>
       <c r="B13" s="2">
-        <v>0.85731228447012064</v>
+        <v>0.85573675100067004</v>
       </c>
       <c r="C13" s="2">
-        <v>0.86067727468320498</v>
+        <v>0.85773064727643067</v>
       </c>
       <c r="D13" s="2">
-        <v>0.86437038851687853</v>
+        <v>0.85848441513750184</v>
       </c>
       <c r="E13" s="2">
-        <v>0.86377979896211154</v>
+        <v>0.86119631930388285</v>
       </c>
       <c r="F13" s="2">
-        <v>0.85866019574214181</v>
+        <v>0.86280632349525188</v>
       </c>
       <c r="G13" s="2">
-        <v>0.8632717590963056</v>
+        <v>0.86275591869981272</v>
       </c>
       <c r="H13" s="2">
-        <v>0.86690496064160205</v>
+        <v>0.86331819516928354</v>
       </c>
       <c r="I13" s="2">
-        <v>0.86048001992952783</v>
+        <v>0.86366631572375652</v>
       </c>
       <c r="J13" s="2">
-        <v>0.85619201266478917</v>
+        <v>0.86243397304631564</v>
       </c>
       <c r="K13" s="2">
-        <v>0.86856724383201034</v>
+        <v>0.86154233992522722</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1016,34 +1014,34 @@
         <v>23</v>
       </c>
       <c r="B15" s="3">
-        <v>109048</v>
+        <v>416408</v>
       </c>
       <c r="C15" s="3">
-        <v>111831</v>
+        <v>427741</v>
       </c>
       <c r="D15" s="3">
-        <v>116429</v>
+        <v>435403</v>
       </c>
       <c r="E15" s="3">
-        <v>120856</v>
+        <v>444857</v>
       </c>
       <c r="F15" s="3">
-        <v>125207</v>
+        <v>458164</v>
       </c>
       <c r="G15" s="3">
-        <v>129627</v>
+        <v>474323</v>
       </c>
       <c r="H15" s="3">
-        <v>134208</v>
+        <v>492119</v>
       </c>
       <c r="I15" s="3">
-        <v>139450</v>
+        <v>509898</v>
       </c>
       <c r="J15" s="3">
-        <v>143671</v>
+        <v>528492</v>
       </c>
       <c r="K15" s="3">
-        <v>145830</v>
+        <v>546956</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1051,34 +1049,34 @@
         <v>24</v>
       </c>
       <c r="B16" s="3">
-        <v>1556</v>
+        <v>7331</v>
       </c>
       <c r="C16" s="3">
-        <v>1618</v>
+        <v>7485</v>
       </c>
       <c r="D16" s="3">
-        <v>1688</v>
+        <v>6898</v>
       </c>
       <c r="E16" s="3">
-        <v>1653</v>
+        <v>6645</v>
       </c>
       <c r="F16" s="3">
-        <v>1601</v>
+        <v>6515</v>
       </c>
       <c r="G16" s="3">
-        <v>1505</v>
+        <v>6560</v>
       </c>
       <c r="H16" s="3">
-        <v>1722</v>
+        <v>6447</v>
       </c>
       <c r="I16" s="3">
-        <v>1746</v>
+        <v>6481</v>
       </c>
       <c r="J16" s="3">
-        <v>1951</v>
+        <v>6574</v>
       </c>
       <c r="K16" s="3">
-        <v>832</v>
+        <v>6924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>